<commit_message>
update start date of measurement tasks
</commit_message>
<xml_diff>
--- a/Project/Project-Schedule.xlsx
+++ b/Project/Project-Schedule.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Schedule-P1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Schedule-P1'!$B$5:$J$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Schedule-P1'!$B$5:$J$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Schedule-P1'!$B$5:$J$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Schedule-P1'!$B$5:$J$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Schedule-P1'!$B$5:$J$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Schedule-P1'!$B$5:$J$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Schedule-P1'!$B$5:$J$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -157,12 +158,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MM\-DD\-YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD\-MM\-YYYY;@"/>
-    <numFmt numFmtId="167" formatCode="0%"/>
-    <numFmt numFmtId="168" formatCode="DD\-MMM\-YYYY;@"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="DD\-MMM\-YYYY;@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -241,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -280,13 +280,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -366,23 +359,23 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,27 +412,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,47 +436,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,11 +468,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -507,7 +484,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,29 +512,29 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.0051020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.86224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -572,7 +549,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -622,297 +599,305 @@
       <c r="F6" s="12" t="n">
         <v>42518</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15" t="s">
+      <c r="G6" s="11" t="n">
+        <v>42517</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="16" t="n">
+      <c r="J6" s="14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="19" t="n">
+      <c r="E7" s="17" t="n">
         <v>42513</v>
       </c>
-      <c r="F7" s="20" t="n">
+      <c r="F7" s="18" t="n">
         <v>42518</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23" t="s">
+      <c r="G7" s="17" t="n">
+        <v>42517</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="17" t="n">
         <v>42519</v>
       </c>
-      <c r="F8" s="20" t="n">
+      <c r="F8" s="18" t="n">
         <v>42531</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23" t="s">
+      <c r="G8" s="17" t="n">
+        <v>42517</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="19" t="n">
+      <c r="E9" s="17" t="n">
         <v>42519</v>
       </c>
-      <c r="F9" s="20" t="n">
+      <c r="F9" s="18" t="n">
         <v>42531</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23" t="s">
+      <c r="G9" s="17" t="n">
+        <v>42517</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="24" t="n">
+      <c r="J9" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="19" t="n">
+      <c r="E10" s="17" t="n">
         <v>42513</v>
       </c>
-      <c r="F10" s="20" t="n">
+      <c r="F10" s="18" t="n">
         <v>42521</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="25" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="24" t="n">
+      <c r="J10" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="19" t="n">
+      <c r="E11" s="17" t="n">
         <v>42513</v>
       </c>
-      <c r="F11" s="20" t="n">
+      <c r="F11" s="18" t="n">
         <v>42521</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="25" t="s">
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="24" t="n">
+      <c r="J11" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="19" t="n">
+      <c r="E12" s="17" t="n">
         <v>42513</v>
       </c>
-      <c r="F12" s="20" t="n">
+      <c r="F12" s="18" t="n">
         <v>42531</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="24" t="n">
+      <c r="J12" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="19" t="n">
+      <c r="E13" s="17" t="n">
         <v>42513</v>
       </c>
-      <c r="F13" s="20" t="n">
+      <c r="F13" s="18" t="n">
         <v>42531</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="19" t="n">
+      <c r="E14" s="17" t="n">
         <v>42532</v>
       </c>
-      <c r="F14" s="20" t="n">
+      <c r="F14" s="18" t="n">
         <v>42541</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="24" t="n">
+      <c r="J14" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="19" t="n">
+      <c r="E15" s="17" t="n">
         <v>42532</v>
       </c>
-      <c r="F15" s="20" t="n">
+      <c r="F15" s="18" t="n">
         <v>42541</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="24" t="n">
+      <c r="J15" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="19" t="n">
+      <c r="E16" s="17" t="n">
         <v>42532</v>
       </c>
-      <c r="F16" s="20" t="n">
+      <c r="F16" s="18" t="n">
         <v>42541</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="24" t="n">
+      <c r="J16" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="35" t="n">
+      <c r="J19" s="31" t="n">
         <f aca="false">AVERAGE(J6:J17)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B5:J15"/>
+  <autoFilter ref="B5:J16"/>
   <mergeCells count="1">
     <mergeCell ref="B2:E3"/>
   </mergeCells>

</xml_diff>